<commit_message>
ajout de model StatisticsData
</commit_message>
<xml_diff>
--- a/statistiques_christelle-borrego_2025-05-05.xlsx
+++ b/statistiques_christelle-borrego_2025-05-05.xlsx
@@ -1,10 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F475511-8829-4411-99BC-EECEF280CC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="8380" yWindow="0" windowWidth="10820" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Statistiques mensuelles" state="visible" r:id="rId4"/>
+    <sheet name="Statistiques mensuelles" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -310,28 +314,36 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -345,13 +357,17 @@
     <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -360,14 +376,16 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -377,6 +395,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,26 +735,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="75" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -887,8 +909,8 @@
       </c>
       <c r="BW2" s="3"/>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="4"/>
@@ -929,8 +951,8 @@
       <c r="BU3" s="4"/>
       <c r="BW3" s="4"/>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="1">
@@ -1082,8 +1104,8 @@
       </c>
       <c r="BW4" s="4"/>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="1">
@@ -1235,8 +1257,8 @@
       </c>
       <c r="BW5" s="4"/>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="1">
@@ -1388,8 +1410,8 @@
       </c>
       <c r="BW6" s="4"/>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="1">
@@ -1541,8 +1563,8 @@
       </c>
       <c r="BW7" s="4"/>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="1">
@@ -1694,8 +1716,8 @@
       </c>
       <c r="BW8" s="4"/>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="1">
@@ -1847,8 +1869,8 @@
       </c>
       <c r="BW9" s="4"/>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="1">
@@ -2000,7 +2022,7 @@
       </c>
       <c r="BW10" s="4"/>
     </row>
-    <row r="11" spans="3:75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.35">
       <c r="C11" s="4"/>
       <c r="E11" s="4"/>
       <c r="G11" s="4"/>
@@ -2039,7 +2061,7 @@
       <c r="BU11" s="4"/>
       <c r="BW11" s="4"/>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -2081,7 +2103,7 @@
       <c r="BU12" s="4"/>
       <c r="BW12" s="4"/>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -2089,7 +2111,7 @@
         <v>208</v>
       </c>
       <c r="C13" s="5">
-        <v>0.3291139240506329</v>
+        <v>0.32911392405063289</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -2143,7 +2165,7 @@
         <v>15</v>
       </c>
       <c r="U13" s="5">
-        <v>0.3191489361702128</v>
+        <v>0.31914893617021278</v>
       </c>
       <c r="V13" s="1">
         <v>0</v>
@@ -2173,7 +2195,7 @@
         <v>21</v>
       </c>
       <c r="AE13" s="5">
-        <v>0.7241379310344828</v>
+        <v>0.72413793103448276</v>
       </c>
       <c r="AF13" s="1">
         <v>0</v>
@@ -2191,7 +2213,7 @@
         <v>9</v>
       </c>
       <c r="AK13" s="5">
-        <v>0.4090909090909091</v>
+        <v>0.40909090909090912</v>
       </c>
       <c r="AL13" s="1">
         <v>0</v>
@@ -2209,19 +2231,19 @@
         <v>12</v>
       </c>
       <c r="AQ13" s="5">
-        <v>0.4444444444444444</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="AR13" s="1">
         <v>8</v>
       </c>
       <c r="AS13" s="5">
-        <v>0.6153846153846154</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="AT13" s="1">
         <v>11</v>
       </c>
       <c r="AU13" s="5">
-        <v>0.2037037037037037</v>
+        <v>0.20370370370370369</v>
       </c>
       <c r="AV13" s="1">
         <v>8</v>
@@ -2263,13 +2285,13 @@
         <v>15</v>
       </c>
       <c r="BI13" s="5">
-        <v>0.4166666666666667</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="BJ13" s="1">
         <v>15</v>
       </c>
       <c r="BK13" s="5">
-        <v>0.3191489361702128</v>
+        <v>0.31914893617021278</v>
       </c>
       <c r="BL13" s="1">
         <v>10</v>
@@ -2281,7 +2303,7 @@
         <v>12</v>
       </c>
       <c r="BO13" s="5">
-        <v>0.2222222222222222</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="BP13" s="1">
         <v>8</v>
@@ -2308,7 +2330,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -2316,7 +2338,7 @@
         <v>424</v>
       </c>
       <c r="C14" s="5">
-        <v>0.6708860759493671</v>
+        <v>0.67088607594936711</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -2364,13 +2386,13 @@
         <v>24</v>
       </c>
       <c r="S14" s="5">
-        <v>0.6486486486486487</v>
+        <v>0.64864864864864868</v>
       </c>
       <c r="T14" s="1">
         <v>32</v>
       </c>
       <c r="U14" s="5">
-        <v>0.6808510638297872</v>
+        <v>0.68085106382978722</v>
       </c>
       <c r="V14" s="1">
         <v>0</v>
@@ -2394,7 +2416,7 @@
         <v>10</v>
       </c>
       <c r="AC14" s="5">
-        <v>0.5263157894736842</v>
+        <v>0.52631578947368418</v>
       </c>
       <c r="AD14" s="1">
         <v>8</v>
@@ -2418,7 +2440,7 @@
         <v>13</v>
       </c>
       <c r="AK14" s="5">
-        <v>0.5909090909090909</v>
+        <v>0.59090909090909094</v>
       </c>
       <c r="AL14" s="1">
         <v>0</v>
@@ -2436,7 +2458,7 @@
         <v>15</v>
       </c>
       <c r="AQ14" s="5">
-        <v>0.5555555555555556</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="AR14" s="1">
         <v>5</v>
@@ -2448,13 +2470,13 @@
         <v>43</v>
       </c>
       <c r="AU14" s="5">
-        <v>0.7962962962962963</v>
+        <v>0.79629629629629628</v>
       </c>
       <c r="AV14" s="1">
         <v>31</v>
       </c>
       <c r="AW14" s="5">
-        <v>0.7948717948717948</v>
+        <v>0.79487179487179482</v>
       </c>
       <c r="AX14" s="1">
         <v>16</v>
@@ -2484,31 +2506,31 @@
         <v>31</v>
       </c>
       <c r="BG14" s="5">
-        <v>0.8611111111111112</v>
+        <v>0.86111111111111116</v>
       </c>
       <c r="BH14" s="1">
         <v>21</v>
       </c>
       <c r="BI14" s="5">
-        <v>0.5833333333333334</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="BJ14" s="1">
         <v>32</v>
       </c>
       <c r="BK14" s="5">
-        <v>0.6808510638297872</v>
+        <v>0.68085106382978722</v>
       </c>
       <c r="BL14" s="1">
         <v>23</v>
       </c>
       <c r="BM14" s="5">
-        <v>0.696969696969697</v>
+        <v>0.69696969696969702</v>
       </c>
       <c r="BN14" s="1">
         <v>42</v>
       </c>
       <c r="BO14" s="5">
-        <v>0.7777777777777778</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="BP14" s="1">
         <v>32</v>
@@ -2535,7 +2557,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -2762,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="3:75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:75" x14ac:dyDescent="0.35">
       <c r="C16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="4"/>
@@ -2801,7 +2823,7 @@
       <c r="BU16" s="4"/>
       <c r="BW16" s="4"/>
     </row>
-    <row r="17" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
@@ -2843,7 +2865,7 @@
       <c r="BU17" s="4"/>
       <c r="BW17" s="4"/>
     </row>
-    <row r="18" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -2863,7 +2885,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="5">
-        <v>0.3333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -2905,7 +2927,7 @@
         <v>1</v>
       </c>
       <c r="U18" s="5">
-        <v>0.03571428571428571</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="V18" s="1">
         <v>3</v>
@@ -2917,7 +2939,7 @@
         <v>2</v>
       </c>
       <c r="Y18" s="5">
-        <v>0.08333333333333333</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="Z18" s="1">
         <v>0</v>
@@ -2935,7 +2957,7 @@
         <v>8</v>
       </c>
       <c r="AE18" s="5">
-        <v>0.2222222222222222</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="AF18" s="1">
         <v>0</v>
@@ -2953,13 +2975,13 @@
         <v>2</v>
       </c>
       <c r="AK18" s="5">
-        <v>0.058823529411764705</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="AL18" s="1">
         <v>2</v>
       </c>
       <c r="AM18" s="5">
-        <v>0.06896551724137931</v>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="AN18" s="1">
         <v>0</v>
@@ -2971,13 +2993,13 @@
         <v>1</v>
       </c>
       <c r="AQ18" s="5">
-        <v>0.038461538461538464</v>
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="AR18" s="1">
         <v>8</v>
       </c>
       <c r="AS18" s="5">
-        <v>0.3076923076923077</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="AT18" s="1">
         <v>6</v>
@@ -2989,7 +3011,7 @@
         <v>2</v>
       </c>
       <c r="AW18" s="5">
-        <v>0.09523809523809523</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="AX18" s="1">
         <v>8</v>
@@ -3007,7 +3029,7 @@
         <v>1</v>
       </c>
       <c r="BC18" s="5">
-        <v>0.043478260869565216</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="BD18" s="1">
         <v>2</v>
@@ -3031,7 +3053,7 @@
         <v>1</v>
       </c>
       <c r="BK18" s="5">
-        <v>0.041666666666666664</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="BL18" s="1">
         <v>2</v>
@@ -3043,7 +3065,7 @@
         <v>1</v>
       </c>
       <c r="BO18" s="5">
-        <v>0.03571428571428571</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="BP18" s="1">
         <v>3</v>
@@ -3070,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -3078,7 +3100,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="5">
-        <v>0.016506189821182942</v>
+        <v>1.6506189821182942E-2</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -3144,7 +3166,7 @@
         <v>1</v>
       </c>
       <c r="Y19" s="5">
-        <v>0.041666666666666664</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="Z19" s="1">
         <v>3</v>
@@ -3156,13 +3178,13 @@
         <v>1</v>
       </c>
       <c r="AC19" s="5">
-        <v>0.023255813953488372</v>
+        <v>2.3255813953488372E-2</v>
       </c>
       <c r="AD19" s="1">
         <v>2</v>
       </c>
       <c r="AE19" s="5">
-        <v>0.05555555555555555</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="AF19" s="1">
         <v>0</v>
@@ -3297,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -3317,7 +3339,7 @@
         <v>4</v>
       </c>
       <c r="G20" s="5">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H20" s="1">
         <v>2</v>
@@ -3335,7 +3357,7 @@
         <v>19</v>
       </c>
       <c r="M20" s="5">
-        <v>0.8636363636363636</v>
+        <v>0.86363636363636365</v>
       </c>
       <c r="N20" s="1">
         <v>22</v>
@@ -3365,7 +3387,7 @@
         <v>23</v>
       </c>
       <c r="W20" s="5">
-        <v>0.8846153846153846</v>
+        <v>0.88461538461538458</v>
       </c>
       <c r="X20" s="1">
         <v>21</v>
@@ -3383,37 +3405,37 @@
         <v>35</v>
       </c>
       <c r="AC20" s="5">
-        <v>0.813953488372093</v>
+        <v>0.81395348837209303</v>
       </c>
       <c r="AD20" s="1">
         <v>26</v>
       </c>
       <c r="AE20" s="5">
-        <v>0.7222222222222222</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="AF20" s="1">
         <v>11</v>
       </c>
       <c r="AG20" s="5">
-        <v>0.9166666666666666</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="AH20" s="1">
         <v>23</v>
       </c>
       <c r="AI20" s="5">
-        <v>0.8518518518518519</v>
+        <v>0.85185185185185186</v>
       </c>
       <c r="AJ20" s="1">
         <v>31</v>
       </c>
       <c r="AK20" s="5">
-        <v>0.9117647058823529</v>
+        <v>0.91176470588235292</v>
       </c>
       <c r="AL20" s="1">
         <v>26</v>
       </c>
       <c r="AM20" s="5">
-        <v>0.896551724137931</v>
+        <v>0.89655172413793105</v>
       </c>
       <c r="AN20" s="1">
         <v>18</v>
@@ -3425,13 +3447,13 @@
         <v>25</v>
       </c>
       <c r="AQ20" s="5">
-        <v>0.9615384615384616</v>
+        <v>0.96153846153846156</v>
       </c>
       <c r="AR20" s="1">
         <v>17</v>
       </c>
       <c r="AS20" s="5">
-        <v>0.6538461538461539</v>
+        <v>0.65384615384615385</v>
       </c>
       <c r="AT20" s="1">
         <v>19</v>
@@ -3443,25 +3465,25 @@
         <v>19</v>
       </c>
       <c r="AW20" s="5">
-        <v>0.9047619047619048</v>
+        <v>0.90476190476190477</v>
       </c>
       <c r="AX20" s="1">
         <v>24</v>
       </c>
       <c r="AY20" s="5">
-        <v>0.631578947368421</v>
+        <v>0.63157894736842102</v>
       </c>
       <c r="AZ20" s="1">
         <v>8</v>
       </c>
       <c r="BA20" s="5">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BB20" s="1">
         <v>18</v>
       </c>
       <c r="BC20" s="5">
-        <v>0.782608695652174</v>
+        <v>0.78260869565217395</v>
       </c>
       <c r="BD20" s="1">
         <v>4</v>
@@ -3479,13 +3501,13 @@
         <v>10</v>
       </c>
       <c r="BI20" s="5">
-        <v>0.4166666666666667</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="BJ20" s="1">
         <v>10</v>
       </c>
       <c r="BK20" s="5">
-        <v>0.4166666666666667</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="BL20" s="1">
         <v>7</v>
@@ -3503,7 +3525,7 @@
         <v>5</v>
       </c>
       <c r="BQ20" s="5">
-        <v>0.2631578947368421</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="BR20" s="1">
         <v>0</v>
@@ -3524,7 +3546,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -3622,7 +3644,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="5">
-        <v>0.08333333333333333</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="AH21" s="1">
         <v>0</v>
@@ -3634,13 +3656,13 @@
         <v>1</v>
       </c>
       <c r="AK21" s="5">
-        <v>0.029411764705882353</v>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="AL21" s="1">
         <v>1</v>
       </c>
       <c r="AM21" s="5">
-        <v>0.034482758620689655</v>
+        <v>3.4482758620689655E-2</v>
       </c>
       <c r="AN21" s="1">
         <v>0</v>
@@ -3658,7 +3680,7 @@
         <v>1</v>
       </c>
       <c r="AS21" s="5">
-        <v>0.038461538461538464</v>
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="AT21" s="1">
         <v>0</v>
@@ -3700,19 +3722,19 @@
         <v>7</v>
       </c>
       <c r="BG21" s="5">
-        <v>0.5384615384615384</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="BH21" s="1">
         <v>14</v>
       </c>
       <c r="BI21" s="5">
-        <v>0.5833333333333334</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="BJ21" s="1">
         <v>13</v>
       </c>
       <c r="BK21" s="5">
-        <v>0.5416666666666666</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="BL21" s="1">
         <v>7</v>
@@ -3730,7 +3752,7 @@
         <v>11</v>
       </c>
       <c r="BQ21" s="5">
-        <v>0.5789473684210527</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="BR21" s="1">
         <v>0</v>
@@ -3751,7 +3773,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="3:75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:75" x14ac:dyDescent="0.35">
       <c r="C22" s="4"/>
       <c r="E22" s="4"/>
       <c r="G22" s="4"/>
@@ -3790,7 +3812,7 @@
       <c r="BU22" s="4"/>
       <c r="BW22" s="4"/>
     </row>
-    <row r="23" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
@@ -3832,7 +3854,7 @@
       <c r="BU23" s="4"/>
       <c r="BW23" s="4"/>
     </row>
-    <row r="24" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3985,7 +4007,7 @@
       </c>
       <c r="BW24" s="4"/>
     </row>
-    <row r="25" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -3993,7 +4015,7 @@
         <v>715</v>
       </c>
       <c r="C25" s="5">
-        <v>0.6126820908311911</v>
+        <v>0.61268209083119107</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -4005,7 +4027,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="5">
-        <v>0.8888888888888888</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="H25" s="1">
         <v>1</v>
@@ -4029,73 +4051,73 @@
         <v>31</v>
       </c>
       <c r="O25" s="5">
-        <v>0.6739130434782609</v>
+        <v>0.67391304347826086</v>
       </c>
       <c r="P25" s="1">
         <v>26</v>
       </c>
       <c r="Q25" s="5">
-        <v>0.6190476190476191</v>
+        <v>0.61904761904761907</v>
       </c>
       <c r="R25" s="1">
         <v>29</v>
       </c>
       <c r="S25" s="5">
-        <v>0.6444444444444445</v>
+        <v>0.64444444444444449</v>
       </c>
       <c r="T25" s="1">
         <v>26</v>
       </c>
       <c r="U25" s="5">
-        <v>0.5306122448979592</v>
+        <v>0.53061224489795922</v>
       </c>
       <c r="V25" s="1">
         <v>22</v>
       </c>
       <c r="W25" s="5">
-        <v>0.4888888888888889</v>
+        <v>0.48888888888888887</v>
       </c>
       <c r="X25" s="1">
         <v>20</v>
       </c>
       <c r="Y25" s="5">
-        <v>0.425531914893617</v>
+        <v>0.42553191489361702</v>
       </c>
       <c r="Z25" s="1">
         <v>33</v>
       </c>
       <c r="AA25" s="5">
-        <v>0.559322033898305</v>
+        <v>0.55932203389830504</v>
       </c>
       <c r="AB25" s="1">
         <v>62</v>
       </c>
       <c r="AC25" s="5">
-        <v>0.8157894736842105</v>
+        <v>0.81578947368421051</v>
       </c>
       <c r="AD25" s="1">
         <v>55</v>
       </c>
       <c r="AE25" s="5">
-        <v>0.873015873015873</v>
+        <v>0.87301587301587302</v>
       </c>
       <c r="AF25" s="1">
         <v>13</v>
       </c>
       <c r="AG25" s="5">
-        <v>0.7647058823529411</v>
+        <v>0.76470588235294112</v>
       </c>
       <c r="AH25" s="1">
         <v>27</v>
       </c>
       <c r="AI25" s="5">
-        <v>0.627906976744186</v>
+        <v>0.62790697674418605</v>
       </c>
       <c r="AJ25" s="1">
         <v>35</v>
       </c>
       <c r="AK25" s="5">
-        <v>0.5932203389830508</v>
+        <v>0.59322033898305082</v>
       </c>
       <c r="AL25" s="1">
         <v>27</v>
@@ -4107,7 +4129,7 @@
         <v>25</v>
       </c>
       <c r="AO25" s="5">
-        <v>0.9259259259259259</v>
+        <v>0.92592592592592593</v>
       </c>
       <c r="AP25" s="1">
         <v>18</v>
@@ -4125,7 +4147,7 @@
         <v>17</v>
       </c>
       <c r="AU25" s="5">
-        <v>0.4146341463414634</v>
+        <v>0.41463414634146339</v>
       </c>
       <c r="AV25" s="1">
         <v>14</v>
@@ -4137,7 +4159,7 @@
         <v>22</v>
       </c>
       <c r="AY25" s="5">
-        <v>0.5238095238095238</v>
+        <v>0.52380952380952384</v>
       </c>
       <c r="AZ25" s="1">
         <v>8</v>
@@ -4179,7 +4201,7 @@
         <v>17</v>
       </c>
       <c r="BM25" s="5">
-        <v>0.5862068965517241</v>
+        <v>0.58620689655172409</v>
       </c>
       <c r="BN25" s="1">
         <v>21</v>
@@ -4191,7 +4213,7 @@
         <v>17</v>
       </c>
       <c r="BQ25" s="5">
-        <v>0.5151515151515151</v>
+        <v>0.51515151515151514</v>
       </c>
       <c r="BR25" s="1">
         <v>1</v>
@@ -4212,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -4220,7 +4242,7 @@
         <v>448</v>
       </c>
       <c r="C26" s="5">
-        <v>0.3838903170522708</v>
+        <v>0.38389031705227078</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -4280,19 +4302,19 @@
         <v>23</v>
       </c>
       <c r="W26" s="5">
-        <v>0.5111111111111111</v>
+        <v>0.51111111111111107</v>
       </c>
       <c r="X26" s="1">
         <v>27</v>
       </c>
       <c r="Y26" s="5">
-        <v>0.574468085106383</v>
+        <v>0.57446808510638303</v>
       </c>
       <c r="Z26" s="1">
         <v>26</v>
       </c>
       <c r="AA26" s="5">
-        <v>0.4406779661016949</v>
+        <v>0.44067796610169491</v>
       </c>
       <c r="AB26" s="1">
         <v>14</v>
@@ -4322,7 +4344,7 @@
         <v>24</v>
       </c>
       <c r="AK26" s="5">
-        <v>0.4067796610169492</v>
+        <v>0.40677966101694918</v>
       </c>
       <c r="AL26" s="1">
         <v>18</v>
@@ -4334,7 +4356,7 @@
         <v>2</v>
       </c>
       <c r="AO26" s="5">
-        <v>0.07407407407407407</v>
+        <v>7.407407407407407E-2</v>
       </c>
       <c r="AP26" s="1">
         <v>24</v>
@@ -4352,7 +4374,7 @@
         <v>24</v>
       </c>
       <c r="AU26" s="5">
-        <v>0.5853658536585366</v>
+        <v>0.58536585365853655</v>
       </c>
       <c r="AV26" s="1">
         <v>14</v>
@@ -4412,7 +4434,7 @@
         <v>32</v>
       </c>
       <c r="BO26" s="5">
-        <v>0.6037735849056604</v>
+        <v>0.60377358490566035</v>
       </c>
       <c r="BP26" s="1">
         <v>16</v>
@@ -4439,7 +4461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -4447,7 +4469,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="5">
-        <v>0.003427592116538132</v>
+        <v>3.4275921165381321E-3</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
@@ -4591,7 +4613,7 @@
         <v>4</v>
       </c>
       <c r="AY27" s="5">
-        <v>0.09523809523809523</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="AZ27" s="1">
         <v>0</v>
@@ -4666,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:75" x14ac:dyDescent="0.35">
       <c r="C28" s="4"/>
       <c r="E28" s="4"/>
       <c r="G28" s="4"/>
@@ -4705,7 +4727,7 @@
       <c r="BU28" s="4"/>
       <c r="BW28" s="4"/>
     </row>
-    <row r="29" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
@@ -4747,7 +4769,7 @@
       <c r="BU29" s="4"/>
       <c r="BW29" s="4"/>
     </row>
-    <row r="30" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -4755,7 +4777,7 @@
         <v>22</v>
       </c>
       <c r="C30" s="5">
-        <v>0.030261348005502064</v>
+        <v>3.0261348005502064E-2</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -4899,7 +4921,7 @@
         <v>2</v>
       </c>
       <c r="AY30" s="5">
-        <v>0.05263157894736842</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="AZ30" s="1">
         <v>2</v>
@@ -4911,7 +4933,7 @@
         <v>12</v>
       </c>
       <c r="BC30" s="5">
-        <v>0.5217391304347826</v>
+        <v>0.52173913043478259</v>
       </c>
       <c r="BD30" s="1">
         <v>0</v>
@@ -4974,7 +4996,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -4982,7 +5004,7 @@
         <v>56</v>
       </c>
       <c r="C31" s="5">
-        <v>0.07702888583218707</v>
+        <v>7.7028885832187075E-2</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
@@ -5108,19 +5130,19 @@
         <v>15</v>
       </c>
       <c r="AS31" s="5">
-        <v>0.5769230769230769</v>
+        <v>0.57692307692307687</v>
       </c>
       <c r="AT31" s="1">
         <v>7</v>
       </c>
       <c r="AU31" s="5">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AV31" s="1">
         <v>2</v>
       </c>
       <c r="AW31" s="5">
-        <v>0.09523809523809523</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="AX31" s="1">
         <v>16</v>
@@ -5132,13 +5154,13 @@
         <v>1</v>
       </c>
       <c r="BA31" s="5">
-        <v>0.08333333333333333</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="BB31" s="1">
         <v>2</v>
       </c>
       <c r="BC31" s="5">
-        <v>0.08695652173913043</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="BD31" s="1">
         <v>1</v>
@@ -5156,7 +5178,7 @@
         <v>1</v>
       </c>
       <c r="BI31" s="5">
-        <v>0.041666666666666664</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="BJ31" s="1">
         <v>0</v>
@@ -5201,7 +5223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -5209,7 +5231,7 @@
         <v>192</v>
       </c>
       <c r="C32" s="5">
-        <v>0.2640990371389271</v>
+        <v>0.26409903713892707</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
@@ -5221,7 +5243,7 @@
         <v>4</v>
       </c>
       <c r="G32" s="5">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H32" s="1">
         <v>2</v>
@@ -5269,19 +5291,19 @@
         <v>7</v>
       </c>
       <c r="W32" s="5">
-        <v>0.2692307692307692</v>
+        <v>0.26923076923076922</v>
       </c>
       <c r="X32" s="1">
         <v>1</v>
       </c>
       <c r="Y32" s="5">
-        <v>0.041666666666666664</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="Z32" s="1">
         <v>1</v>
       </c>
       <c r="AA32" s="5">
-        <v>0.03333333333333333</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="AB32" s="1">
         <v>10</v>
@@ -5293,19 +5315,19 @@
         <v>10</v>
       </c>
       <c r="AE32" s="5">
-        <v>0.2777777777777778</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="AF32" s="1">
         <v>7</v>
       </c>
       <c r="AG32" s="5">
-        <v>0.5833333333333334</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="AH32" s="1">
         <v>11</v>
       </c>
       <c r="AI32" s="5">
-        <v>0.4074074074074074</v>
+        <v>0.40740740740740738</v>
       </c>
       <c r="AJ32" s="1">
         <v>12</v>
@@ -5317,13 +5339,13 @@
         <v>14</v>
       </c>
       <c r="AM32" s="5">
-        <v>0.4827586206896552</v>
+        <v>0.48275862068965519</v>
       </c>
       <c r="AN32" s="1">
         <v>10</v>
       </c>
       <c r="AO32" s="5">
-        <v>0.5555555555555556</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="AP32" s="1">
         <v>3</v>
@@ -5347,13 +5369,13 @@
         <v>2</v>
       </c>
       <c r="AW32" s="5">
-        <v>0.09523809523809523</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="AX32" s="1">
         <v>10</v>
       </c>
       <c r="AY32" s="5">
-        <v>0.2631578947368421</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="AZ32" s="1">
         <v>9</v>
@@ -5365,7 +5387,7 @@
         <v>9</v>
       </c>
       <c r="BC32" s="5">
-        <v>0.391304347826087</v>
+        <v>0.39130434782608697</v>
       </c>
       <c r="BD32" s="1">
         <v>6</v>
@@ -5383,7 +5405,7 @@
         <v>7</v>
       </c>
       <c r="BI32" s="5">
-        <v>0.2916666666666667</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="BJ32" s="1">
         <v>3</v>
@@ -5428,7 +5450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -5436,7 +5458,7 @@
         <v>457</v>
       </c>
       <c r="C33" s="5">
-        <v>0.6286107290233838</v>
+        <v>0.62861072902338377</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
@@ -5448,7 +5470,7 @@
         <v>2</v>
       </c>
       <c r="G33" s="5">
-        <v>0.3333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H33" s="1">
         <v>0</v>
@@ -5466,7 +5488,7 @@
         <v>18</v>
       </c>
       <c r="M33" s="5">
-        <v>0.8181818181818182</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="N33" s="1">
         <v>19</v>
@@ -5484,7 +5506,7 @@
         <v>20</v>
       </c>
       <c r="S33" s="5">
-        <v>0.8333333333333334</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="T33" s="1">
         <v>20</v>
@@ -5496,43 +5518,43 @@
         <v>19</v>
       </c>
       <c r="W33" s="5">
-        <v>0.7307692307692307</v>
+        <v>0.73076923076923073</v>
       </c>
       <c r="X33" s="1">
         <v>23</v>
       </c>
       <c r="Y33" s="5">
-        <v>0.9583333333333334</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="Z33" s="1">
         <v>29</v>
       </c>
       <c r="AA33" s="5">
-        <v>0.9666666666666667</v>
+        <v>0.96666666666666667</v>
       </c>
       <c r="AB33" s="1">
         <v>33</v>
       </c>
       <c r="AC33" s="5">
-        <v>0.7674418604651163</v>
+        <v>0.76744186046511631</v>
       </c>
       <c r="AD33" s="1">
         <v>26</v>
       </c>
       <c r="AE33" s="5">
-        <v>0.7222222222222222</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="AF33" s="1">
         <v>5</v>
       </c>
       <c r="AG33" s="5">
-        <v>0.4166666666666667</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="AH33" s="1">
         <v>16</v>
       </c>
       <c r="AI33" s="5">
-        <v>0.5925925925925926</v>
+        <v>0.59259259259259256</v>
       </c>
       <c r="AJ33" s="1">
         <v>22</v>
@@ -5544,19 +5566,19 @@
         <v>15</v>
       </c>
       <c r="AM33" s="5">
-        <v>0.5172413793103449</v>
+        <v>0.51724137931034486</v>
       </c>
       <c r="AN33" s="1">
         <v>8</v>
       </c>
       <c r="AO33" s="5">
-        <v>0.4444444444444444</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="AP33" s="1">
         <v>17</v>
       </c>
       <c r="AQ33" s="5">
-        <v>0.6538461538461539</v>
+        <v>0.65384615384615385</v>
       </c>
       <c r="AR33" s="1">
         <v>5</v>
@@ -5580,7 +5602,7 @@
         <v>10</v>
       </c>
       <c r="AY33" s="5">
-        <v>0.2631578947368421</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="AZ33" s="1">
         <v>0</v>
@@ -5604,13 +5626,13 @@
         <v>11</v>
       </c>
       <c r="BG33" s="5">
-        <v>0.8461538461538461</v>
+        <v>0.84615384615384615</v>
       </c>
       <c r="BH33" s="1">
         <v>16</v>
       </c>
       <c r="BI33" s="5">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="BJ33" s="1">
         <v>21</v>
@@ -5634,7 +5656,7 @@
         <v>14</v>
       </c>
       <c r="BQ33" s="5">
-        <v>0.7368421052631579</v>
+        <v>0.73684210526315785</v>
       </c>
       <c r="BR33" s="1">
         <v>0</v>
@@ -5655,7 +5677,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="3:75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:75" x14ac:dyDescent="0.35">
       <c r="C34" s="4"/>
       <c r="E34" s="4"/>
       <c r="G34" s="4"/>
@@ -5694,7 +5716,7 @@
       <c r="BU34" s="4"/>
       <c r="BW34" s="4"/>
     </row>
-    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
@@ -5736,7 +5758,7 @@
       <c r="BU35" s="4"/>
       <c r="BW35" s="4"/>
     </row>
-    <row r="36" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -5963,7 +5985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -5971,7 +5993,7 @@
         <v>9</v>
       </c>
       <c r="C37" s="5">
-        <v>0.006189821182943604</v>
+        <v>6.1898211829436037E-3</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -6079,7 +6101,7 @@
         <v>4</v>
       </c>
       <c r="AM37" s="5">
-        <v>0.04938271604938271</v>
+        <v>4.9382716049382713E-2</v>
       </c>
       <c r="AN37" s="1">
         <v>0</v>
@@ -6103,7 +6125,7 @@
         <v>4</v>
       </c>
       <c r="AU37" s="5">
-        <v>0.057971014492753624</v>
+        <v>5.7971014492753624E-2</v>
       </c>
       <c r="AV37" s="1">
         <v>0</v>
@@ -6145,7 +6167,7 @@
         <v>1</v>
       </c>
       <c r="BI37" s="5">
-        <v>0.02702702702702703</v>
+        <v>2.7027027027027029E-2</v>
       </c>
       <c r="BJ37" s="1">
         <v>0</v>
@@ -6190,7 +6212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -6198,7 +6220,7 @@
         <v>80</v>
       </c>
       <c r="C38" s="5">
-        <v>0.055020632737276476</v>
+        <v>5.5020632737276476E-2</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
@@ -6228,7 +6250,7 @@
         <v>2</v>
       </c>
       <c r="M38" s="5">
-        <v>0.05555555555555555</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="N38" s="1">
         <v>0</v>
@@ -6240,19 +6262,19 @@
         <v>1</v>
       </c>
       <c r="Q38" s="5">
-        <v>0.021739130434782608</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="R38" s="1">
         <v>1</v>
       </c>
       <c r="S38" s="5">
-        <v>0.02564102564102564</v>
+        <v>2.564102564102564E-2</v>
       </c>
       <c r="T38" s="1">
         <v>3</v>
       </c>
       <c r="U38" s="5">
-        <v>0.047619047619047616</v>
+        <v>4.7619047619047616E-2</v>
       </c>
       <c r="V38" s="1">
         <v>0</v>
@@ -6264,7 +6286,7 @@
         <v>1</v>
       </c>
       <c r="Y38" s="5">
-        <v>0.017543859649122806</v>
+        <v>1.7543859649122806E-2</v>
       </c>
       <c r="Z38" s="1">
         <v>0</v>
@@ -6276,37 +6298,37 @@
         <v>5</v>
       </c>
       <c r="AC38" s="5">
-        <v>0.08196721311475409</v>
+        <v>8.1967213114754092E-2</v>
       </c>
       <c r="AD38" s="1">
         <v>1</v>
       </c>
       <c r="AE38" s="5">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AF38" s="1">
         <v>1</v>
       </c>
       <c r="AG38" s="5">
-        <v>0.043478260869565216</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="AH38" s="1">
         <v>19</v>
       </c>
       <c r="AI38" s="5">
-        <v>0.1958762886597938</v>
+        <v>0.19587628865979381</v>
       </c>
       <c r="AJ38" s="1">
         <v>3</v>
       </c>
       <c r="AK38" s="5">
-        <v>0.03571428571428571</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="AL38" s="1">
         <v>7</v>
       </c>
       <c r="AM38" s="5">
-        <v>0.08641975308641975</v>
+        <v>8.6419753086419748E-2</v>
       </c>
       <c r="AN38" s="1">
         <v>4</v>
@@ -6318,19 +6340,19 @@
         <v>4</v>
       </c>
       <c r="AQ38" s="5">
-        <v>0.056338028169014086</v>
+        <v>5.6338028169014086E-2</v>
       </c>
       <c r="AR38" s="1">
         <v>2</v>
       </c>
       <c r="AS38" s="5">
-        <v>0.058823529411764705</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="AT38" s="1">
         <v>3</v>
       </c>
       <c r="AU38" s="5">
-        <v>0.043478260869565216</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="AV38" s="1">
         <v>6</v>
@@ -6342,7 +6364,7 @@
         <v>6</v>
       </c>
       <c r="AY38" s="5">
-        <v>0.09230769230769231</v>
+        <v>9.2307692307692313E-2</v>
       </c>
       <c r="AZ38" s="1">
         <v>0</v>
@@ -6354,7 +6376,7 @@
         <v>1</v>
       </c>
       <c r="BC38" s="5">
-        <v>0.043478260869565216</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="BD38" s="1">
         <v>0</v>
@@ -6384,13 +6406,13 @@
         <v>1</v>
       </c>
       <c r="BM38" s="5">
-        <v>0.030303030303030304</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="BN38" s="1">
         <v>3</v>
       </c>
       <c r="BO38" s="5">
-        <v>0.05357142857142857</v>
+        <v>5.3571428571428568E-2</v>
       </c>
       <c r="BP38" s="1">
         <v>0</v>
@@ -6417,7 +6439,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -6425,7 +6447,7 @@
         <v>915</v>
       </c>
       <c r="C39" s="5">
-        <v>0.6292984869325997</v>
+        <v>0.62929848693259971</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
@@ -6443,7 +6465,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="5">
-        <v>0.6153846153846154</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="J39" s="1">
         <v>2</v>
@@ -6455,13 +6477,13 @@
         <v>15</v>
       </c>
       <c r="M39" s="5">
-        <v>0.4166666666666667</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="N39" s="1">
         <v>21</v>
       </c>
       <c r="O39" s="5">
-        <v>0.5675675675675675</v>
+        <v>0.56756756756756754</v>
       </c>
       <c r="P39" s="1">
         <v>23</v>
@@ -6473,13 +6495,13 @@
         <v>24</v>
       </c>
       <c r="S39" s="5">
-        <v>0.6153846153846154</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="T39" s="1">
         <v>39</v>
       </c>
       <c r="U39" s="5">
-        <v>0.6190476190476191</v>
+        <v>0.61904761904761907</v>
       </c>
       <c r="V39" s="1">
         <v>52</v>
@@ -6491,13 +6513,13 @@
         <v>29</v>
       </c>
       <c r="Y39" s="5">
-        <v>0.5087719298245614</v>
+        <v>0.50877192982456143</v>
       </c>
       <c r="Z39" s="1">
         <v>42</v>
       </c>
       <c r="AA39" s="5">
-        <v>0.7777777777777778</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="AB39" s="1">
         <v>36</v>
@@ -6515,25 +6537,25 @@
         <v>16</v>
       </c>
       <c r="AG39" s="5">
-        <v>0.6956521739130435</v>
+        <v>0.69565217391304346</v>
       </c>
       <c r="AH39" s="1">
         <v>58</v>
       </c>
       <c r="AI39" s="5">
-        <v>0.5979381443298969</v>
+        <v>0.59793814432989689</v>
       </c>
       <c r="AJ39" s="1">
         <v>53</v>
       </c>
       <c r="AK39" s="5">
-        <v>0.6309523809523809</v>
+        <v>0.63095238095238093</v>
       </c>
       <c r="AL39" s="1">
         <v>36</v>
       </c>
       <c r="AM39" s="5">
-        <v>0.4444444444444444</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="AN39" s="1">
         <v>6</v>
@@ -6545,25 +6567,25 @@
         <v>61</v>
       </c>
       <c r="AQ39" s="5">
-        <v>0.8591549295774648</v>
+        <v>0.85915492957746475</v>
       </c>
       <c r="AR39" s="1">
         <v>19</v>
       </c>
       <c r="AS39" s="5">
-        <v>0.5588235294117647</v>
+        <v>0.55882352941176472</v>
       </c>
       <c r="AT39" s="1">
         <v>46</v>
       </c>
       <c r="AU39" s="5">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AV39" s="1">
         <v>34</v>
       </c>
       <c r="AW39" s="5">
-        <v>0.7555555555555555</v>
+        <v>0.75555555555555554</v>
       </c>
       <c r="AX39" s="1">
         <v>23</v>
@@ -6575,13 +6597,13 @@
         <v>12</v>
       </c>
       <c r="BA39" s="5">
-        <v>0.7058823529411765</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="BB39" s="1">
         <v>12</v>
       </c>
       <c r="BC39" s="5">
-        <v>0.5217391304347826</v>
+        <v>0.52173913043478259</v>
       </c>
       <c r="BD39" s="1">
         <v>0</v>
@@ -6593,25 +6615,25 @@
         <v>57</v>
       </c>
       <c r="BG39" s="5">
-        <v>0.9661016949152542</v>
+        <v>0.96610169491525422</v>
       </c>
       <c r="BH39" s="1">
         <v>27</v>
       </c>
       <c r="BI39" s="5">
-        <v>0.7297297297297297</v>
+        <v>0.72972972972972971</v>
       </c>
       <c r="BJ39" s="1">
         <v>39</v>
       </c>
       <c r="BK39" s="5">
-        <v>0.8297872340425532</v>
+        <v>0.82978723404255317</v>
       </c>
       <c r="BL39" s="1">
         <v>24</v>
       </c>
       <c r="BM39" s="5">
-        <v>0.7272727272727273</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="BN39" s="1">
         <v>43</v>
@@ -6644,7 +6666,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="40" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -6664,7 +6686,7 @@
         <v>15</v>
       </c>
       <c r="G40" s="5">
-        <v>0.8823529411764706</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="H40" s="1">
         <v>5</v>
@@ -6682,7 +6704,7 @@
         <v>19</v>
       </c>
       <c r="M40" s="5">
-        <v>0.5277777777777778</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="N40" s="1">
         <v>16</v>
@@ -6694,19 +6716,19 @@
         <v>22</v>
       </c>
       <c r="Q40" s="5">
-        <v>0.4782608695652174</v>
+        <v>0.47826086956521741</v>
       </c>
       <c r="R40" s="1">
         <v>14</v>
       </c>
       <c r="S40" s="5">
-        <v>0.358974358974359</v>
+        <v>0.35897435897435898</v>
       </c>
       <c r="T40" s="1">
         <v>21</v>
       </c>
       <c r="U40" s="5">
-        <v>0.3333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="V40" s="1">
         <v>12</v>
@@ -6724,7 +6746,7 @@
         <v>12</v>
       </c>
       <c r="AA40" s="5">
-        <v>0.2222222222222222</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="AB40" s="1">
         <v>20</v>
@@ -6754,7 +6776,7 @@
         <v>28</v>
       </c>
       <c r="AK40" s="5">
-        <v>0.3333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AL40" s="1">
         <v>34</v>
@@ -6772,7 +6794,7 @@
         <v>6</v>
       </c>
       <c r="AQ40" s="5">
-        <v>0.08450704225352113</v>
+        <v>8.4507042253521125E-2</v>
       </c>
       <c r="AR40" s="1">
         <v>13</v>
@@ -6796,7 +6818,7 @@
         <v>36</v>
       </c>
       <c r="AY40" s="5">
-        <v>0.5538461538461539</v>
+        <v>0.55384615384615388</v>
       </c>
       <c r="AZ40" s="1">
         <v>5</v>
@@ -6820,7 +6842,7 @@
         <v>2</v>
       </c>
       <c r="BG40" s="5">
-        <v>0.03389830508474576</v>
+        <v>3.3898305084745763E-2</v>
       </c>
       <c r="BH40" s="1">
         <v>4</v>
@@ -6871,7 +6893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:75" x14ac:dyDescent="0.35">
       <c r="C41" s="4"/>
       <c r="E41" s="4"/>
       <c r="G41" s="4"/>
@@ -6910,7 +6932,7 @@
       <c r="BU41" s="4"/>
       <c r="BW41" s="4"/>
     </row>
-    <row r="42" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>72</v>
       </c>
@@ -6952,7 +6974,7 @@
       <c r="BU42" s="4"/>
       <c r="BW42" s="4"/>
     </row>
-    <row r="43" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>73</v>
       </c>
@@ -6960,7 +6982,7 @@
         <v>11</v>
       </c>
       <c r="C43" s="5">
-        <v>0.007565337001375516</v>
+        <v>7.5653370013755161E-3</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
@@ -7068,7 +7090,7 @@
         <v>2</v>
       </c>
       <c r="AM43" s="5">
-        <v>0.024691358024691357</v>
+        <v>2.4691358024691357E-2</v>
       </c>
       <c r="AN43" s="1">
         <v>0</v>
@@ -7092,7 +7114,7 @@
         <v>4</v>
       </c>
       <c r="AU43" s="5">
-        <v>0.057971014492753624</v>
+        <v>5.7971014492753624E-2</v>
       </c>
       <c r="AV43" s="1">
         <v>5</v>
@@ -7179,7 +7201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -7217,7 +7239,7 @@
         <v>11</v>
       </c>
       <c r="M44" s="5">
-        <v>0.3055555555555556</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="N44" s="1">
         <v>14</v>
@@ -7253,7 +7275,7 @@
         <v>5</v>
       </c>
       <c r="Y44" s="5">
-        <v>0.08771929824561403</v>
+        <v>8.771929824561403E-2</v>
       </c>
       <c r="Z44" s="1">
         <v>7</v>
@@ -7265,7 +7287,7 @@
         <v>27</v>
       </c>
       <c r="AC44" s="5">
-        <v>0.4426229508196721</v>
+        <v>0.44262295081967212</v>
       </c>
       <c r="AD44" s="1">
         <v>10</v>
@@ -7283,13 +7305,13 @@
         <v>6</v>
       </c>
       <c r="AI44" s="5">
-        <v>0.061855670103092786</v>
+        <v>6.1855670103092786E-2</v>
       </c>
       <c r="AJ44" s="1">
         <v>19</v>
       </c>
       <c r="AK44" s="5">
-        <v>0.2261904761904762</v>
+        <v>0.22619047619047619</v>
       </c>
       <c r="AL44" s="1">
         <v>11</v>
@@ -7307,7 +7329,7 @@
         <v>1</v>
       </c>
       <c r="AQ44" s="5">
-        <v>0.014084507042253521</v>
+        <v>1.4084507042253521E-2</v>
       </c>
       <c r="AR44" s="1">
         <v>5</v>
@@ -7331,7 +7353,7 @@
         <v>6</v>
       </c>
       <c r="AY44" s="5">
-        <v>0.09230769230769231</v>
+        <v>9.2307692307692313E-2</v>
       </c>
       <c r="AZ44" s="1">
         <v>5</v>
@@ -7355,13 +7377,13 @@
         <v>55</v>
       </c>
       <c r="BG44" s="5">
-        <v>0.9322033898305084</v>
+        <v>0.93220338983050843</v>
       </c>
       <c r="BH44" s="1">
         <v>33</v>
       </c>
       <c r="BI44" s="5">
-        <v>0.8918918918918919</v>
+        <v>0.89189189189189189</v>
       </c>
       <c r="BJ44" s="1">
         <v>19</v>
@@ -7385,7 +7407,7 @@
         <v>23</v>
       </c>
       <c r="BQ44" s="5">
-        <v>0.575</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="BR44" s="1">
         <v>0</v>
@@ -7406,7 +7428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -7456,31 +7478,31 @@
         <v>4</v>
       </c>
       <c r="Q45" s="5">
-        <v>0.08695652173913043</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="R45" s="1">
         <v>5</v>
       </c>
       <c r="S45" s="5">
-        <v>0.1282051282051282</v>
+        <v>0.12820512820512819</v>
       </c>
       <c r="T45" s="1">
         <v>5</v>
       </c>
       <c r="U45" s="5">
-        <v>0.07936507936507936</v>
+        <v>7.9365079365079361E-2</v>
       </c>
       <c r="V45" s="1">
         <v>5</v>
       </c>
       <c r="W45" s="5">
-        <v>0.078125</v>
+        <v>7.8125E-2</v>
       </c>
       <c r="X45" s="1">
         <v>4</v>
       </c>
       <c r="Y45" s="5">
-        <v>0.07017543859649122</v>
+        <v>7.0175438596491224E-2</v>
       </c>
       <c r="Z45" s="1">
         <v>8</v>
@@ -7492,31 +7514,31 @@
         <v>4</v>
       </c>
       <c r="AC45" s="5">
-        <v>0.06557377049180328</v>
+        <v>6.5573770491803282E-2</v>
       </c>
       <c r="AD45" s="1">
         <v>7</v>
       </c>
       <c r="AE45" s="5">
-        <v>0.175</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="AF45" s="1">
         <v>1</v>
       </c>
       <c r="AG45" s="5">
-        <v>0.043478260869565216</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="AH45" s="1">
         <v>2</v>
       </c>
       <c r="AI45" s="5">
-        <v>0.020618556701030927</v>
+        <v>2.0618556701030927E-2</v>
       </c>
       <c r="AJ45" s="1">
         <v>8</v>
       </c>
       <c r="AK45" s="5">
-        <v>0.09523809523809523</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="AL45" s="1">
         <v>10</v>
@@ -7534,7 +7556,7 @@
         <v>6</v>
       </c>
       <c r="AQ45" s="5">
-        <v>0.08450704225352113</v>
+        <v>8.4507042253521125E-2</v>
       </c>
       <c r="AR45" s="1">
         <v>10</v>
@@ -7558,7 +7580,7 @@
         <v>20</v>
       </c>
       <c r="AY45" s="5">
-        <v>0.3076923076923077</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="AZ45" s="1">
         <v>3</v>
@@ -7582,7 +7604,7 @@
         <v>2</v>
       </c>
       <c r="BG45" s="5">
-        <v>0.03389830508474576</v>
+        <v>3.3898305084745763E-2</v>
       </c>
       <c r="BH45" s="1">
         <v>0</v>
@@ -7594,7 +7616,7 @@
         <v>4</v>
       </c>
       <c r="BK45" s="5">
-        <v>0.0851063829787234</v>
+        <v>8.5106382978723402E-2</v>
       </c>
       <c r="BL45" s="1">
         <v>4</v>
@@ -7612,7 +7634,7 @@
         <v>9</v>
       </c>
       <c r="BQ45" s="5">
-        <v>0.225</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="BR45" s="1">
         <v>0</v>
@@ -7633,7 +7655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -7641,7 +7663,7 @@
         <v>417</v>
       </c>
       <c r="C46" s="5">
-        <v>0.2867950481430536</v>
+        <v>0.28679504814305362</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
@@ -7671,13 +7693,13 @@
         <v>19</v>
       </c>
       <c r="M46" s="5">
-        <v>0.5277777777777778</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="N46" s="1">
         <v>19</v>
       </c>
       <c r="O46" s="5">
-        <v>0.5135135135135135</v>
+        <v>0.51351351351351349</v>
       </c>
       <c r="P46" s="1">
         <v>14</v>
@@ -7689,7 +7711,7 @@
         <v>14</v>
       </c>
       <c r="S46" s="5">
-        <v>0.358974358974359</v>
+        <v>0.35897435897435898</v>
       </c>
       <c r="T46" s="1">
         <v>13</v>
@@ -7713,7 +7735,7 @@
         <v>11</v>
       </c>
       <c r="AA46" s="5">
-        <v>0.2037037037037037</v>
+        <v>0.20370370370370369</v>
       </c>
       <c r="AB46" s="1">
         <v>16</v>
@@ -7725,7 +7747,7 @@
         <v>23</v>
       </c>
       <c r="AE46" s="5">
-        <v>0.575</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="AF46" s="1">
         <v>6</v>
@@ -7743,7 +7765,7 @@
         <v>22</v>
       </c>
       <c r="AK46" s="5">
-        <v>0.2619047619047619</v>
+        <v>0.26190476190476192</v>
       </c>
       <c r="AL46" s="1">
         <v>29</v>
@@ -7761,7 +7783,7 @@
         <v>4</v>
       </c>
       <c r="AQ46" s="5">
-        <v>0.056338028169014086</v>
+        <v>5.6338028169014086E-2</v>
       </c>
       <c r="AR46" s="1">
         <v>13</v>
@@ -7785,13 +7807,13 @@
         <v>37</v>
       </c>
       <c r="AY46" s="5">
-        <v>0.5692307692307692</v>
+        <v>0.56923076923076921</v>
       </c>
       <c r="AZ46" s="1">
         <v>9</v>
       </c>
       <c r="BA46" s="5">
-        <v>0.5294117647058824</v>
+        <v>0.52941176470588236</v>
       </c>
       <c r="BB46" s="1">
         <v>10</v>
@@ -7809,7 +7831,7 @@
         <v>2</v>
       </c>
       <c r="BG46" s="5">
-        <v>0.03389830508474576</v>
+        <v>3.3898305084745763E-2</v>
       </c>
       <c r="BH46" s="1">
         <v>4</v>
@@ -7821,7 +7843,7 @@
         <v>17</v>
       </c>
       <c r="BK46" s="5">
-        <v>0.3617021276595745</v>
+        <v>0.36170212765957449</v>
       </c>
       <c r="BL46" s="1">
         <v>8</v>
@@ -7860,7 +7882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -7880,7 +7902,7 @@
         <v>12</v>
       </c>
       <c r="G47" s="5">
-        <v>0.7058823529411765</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="H47" s="1">
         <v>2</v>
@@ -7916,7 +7938,7 @@
         <v>1</v>
       </c>
       <c r="S47" s="5">
-        <v>0.02564102564102564</v>
+        <v>2.564102564102564E-2</v>
       </c>
       <c r="T47" s="1">
         <v>20</v>
@@ -7940,7 +7962,7 @@
         <v>28</v>
       </c>
       <c r="AA47" s="5">
-        <v>0.5185185185185185</v>
+        <v>0.51851851851851849</v>
       </c>
       <c r="AB47" s="1">
         <v>14</v>
@@ -7958,19 +7980,19 @@
         <v>11</v>
       </c>
       <c r="AG47" s="5">
-        <v>0.4782608695652174</v>
+        <v>0.47826086956521741</v>
       </c>
       <c r="AH47" s="1">
         <v>79</v>
       </c>
       <c r="AI47" s="5">
-        <v>0.8144329896907216</v>
+        <v>0.81443298969072164</v>
       </c>
       <c r="AJ47" s="1">
         <v>35</v>
       </c>
       <c r="AK47" s="5">
-        <v>0.4166666666666667</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="AL47" s="1">
         <v>29</v>
@@ -7988,7 +8010,7 @@
         <v>60</v>
       </c>
       <c r="AQ47" s="5">
-        <v>0.8450704225352113</v>
+        <v>0.84507042253521125</v>
       </c>
       <c r="AR47" s="1">
         <v>6</v>
@@ -8000,19 +8022,19 @@
         <v>23</v>
       </c>
       <c r="AU47" s="5">
-        <v>0.3333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AV47" s="1">
         <v>22</v>
       </c>
       <c r="AW47" s="5">
-        <v>0.4888888888888889</v>
+        <v>0.48888888888888887</v>
       </c>
       <c r="AX47" s="1">
         <v>2</v>
       </c>
       <c r="AY47" s="5">
-        <v>0.03076923076923077</v>
+        <v>3.0769230769230771E-2</v>
       </c>
       <c r="AZ47" s="1">
         <v>0</v>
@@ -8054,7 +8076,7 @@
         <v>11</v>
       </c>
       <c r="BM47" s="5">
-        <v>0.3333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="BN47" s="1">
         <v>0</v>
@@ -8087,7 +8109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:75" x14ac:dyDescent="0.35">
       <c r="C48" s="4"/>
       <c r="E48" s="4"/>
       <c r="G48" s="4"/>
@@ -8126,7 +8148,7 @@
       <c r="BU48" s="4"/>
       <c r="BW48" s="4"/>
     </row>
-    <row r="49" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>78</v>
       </c>
@@ -8168,7 +8190,7 @@
       <c r="BU49" s="4"/>
       <c r="BW49" s="4"/>
     </row>
-    <row r="50" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -8176,7 +8198,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="5">
-        <v>0.0007374631268436578</v>
+        <v>7.3746312684365781E-4</v>
       </c>
       <c r="D50" s="1">
         <v>0</v>
@@ -8368,7 +8390,7 @@
         <v>1</v>
       </c>
       <c r="BO50" s="5">
-        <v>0.020833333333333332</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="BP50" s="1">
         <v>0</v>
@@ -8395,7 +8417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -8403,7 +8425,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="5">
-        <v>0.0014749262536873156</v>
+        <v>1.4749262536873156E-3</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
@@ -8469,7 +8491,7 @@
         <v>2</v>
       </c>
       <c r="Y51" s="5">
-        <v>0.041666666666666664</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="Z51" s="1">
         <v>0</v>
@@ -8622,7 +8644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>81</v>
       </c>
@@ -8690,7 +8712,7 @@
         <v>3</v>
       </c>
       <c r="W52" s="5">
-        <v>0.08108108108108109</v>
+        <v>8.1081081081081086E-2</v>
       </c>
       <c r="X52" s="1">
         <v>11</v>
@@ -8732,7 +8754,7 @@
         <v>16</v>
       </c>
       <c r="AK52" s="5">
-        <v>0.2077922077922078</v>
+        <v>0.20779220779220781</v>
       </c>
       <c r="AL52" s="1">
         <v>7</v>
@@ -8744,7 +8766,7 @@
         <v>3</v>
       </c>
       <c r="AO52" s="5">
-        <v>0.09375</v>
+        <v>9.375E-2</v>
       </c>
       <c r="AP52" s="1">
         <v>13</v>
@@ -8756,13 +8778,13 @@
         <v>3</v>
       </c>
       <c r="AS52" s="5">
-        <v>0.0625</v>
+        <v>6.25E-2</v>
       </c>
       <c r="AT52" s="1">
         <v>2</v>
       </c>
       <c r="AU52" s="5">
-        <v>0.038461538461538464</v>
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="AV52" s="1">
         <v>0</v>
@@ -8810,7 +8832,7 @@
         <v>1</v>
       </c>
       <c r="BK52" s="5">
-        <v>0.03125</v>
+        <v>3.125E-2</v>
       </c>
       <c r="BL52" s="1">
         <v>0</v>
@@ -8822,7 +8844,7 @@
         <v>1</v>
       </c>
       <c r="BO52" s="5">
-        <v>0.020833333333333332</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="BP52" s="1">
         <v>0</v>
@@ -8849,7 +8871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>82</v>
       </c>
@@ -8857,7 +8879,7 @@
         <v>26</v>
       </c>
       <c r="C53" s="5">
-        <v>0.019174041297935103</v>
+        <v>1.9174041297935103E-2</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
@@ -8941,7 +8963,7 @@
         <v>3</v>
       </c>
       <c r="AE53" s="5">
-        <v>0.03296703296703297</v>
+        <v>3.2967032967032968E-2</v>
       </c>
       <c r="AF53" s="1">
         <v>0</v>
@@ -8953,13 +8975,13 @@
         <v>3</v>
       </c>
       <c r="AI53" s="5">
-        <v>0.05454545454545454</v>
+        <v>5.4545454545454543E-2</v>
       </c>
       <c r="AJ53" s="1">
         <v>4</v>
       </c>
       <c r="AK53" s="5">
-        <v>0.05194805194805195</v>
+        <v>5.1948051948051951E-2</v>
       </c>
       <c r="AL53" s="1">
         <v>0</v>
@@ -8995,13 +9017,13 @@
         <v>3</v>
       </c>
       <c r="AW53" s="5">
-        <v>0.06521739130434782</v>
+        <v>6.5217391304347824E-2</v>
       </c>
       <c r="AX53" s="1">
         <v>1</v>
       </c>
       <c r="AY53" s="5">
-        <v>0.016129032258064516</v>
+        <v>1.6129032258064516E-2</v>
       </c>
       <c r="AZ53" s="1">
         <v>0</v>
@@ -9043,13 +9065,13 @@
         <v>1</v>
       </c>
       <c r="BM53" s="5">
-        <v>0.03333333333333333</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="BN53" s="1">
         <v>4</v>
       </c>
       <c r="BO53" s="5">
-        <v>0.08333333333333333</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="BP53" s="1">
         <v>0</v>
@@ -9067,7 +9089,7 @@
         <v>1</v>
       </c>
       <c r="BU53" s="5">
-        <v>0.06666666666666667</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="BV53" s="1">
         <v>0</v>
@@ -9076,7 +9098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>83</v>
       </c>
@@ -9084,7 +9106,7 @@
         <v>6</v>
       </c>
       <c r="C54" s="5">
-        <v>0.004424778761061947</v>
+        <v>4.4247787610619468E-3</v>
       </c>
       <c r="D54" s="1">
         <v>0</v>
@@ -9168,7 +9190,7 @@
         <v>1</v>
       </c>
       <c r="AE54" s="5">
-        <v>0.01098901098901099</v>
+        <v>1.098901098901099E-2</v>
       </c>
       <c r="AF54" s="1">
         <v>0</v>
@@ -9180,13 +9202,13 @@
         <v>2</v>
       </c>
       <c r="AI54" s="5">
-        <v>0.03636363636363636</v>
+        <v>3.6363636363636362E-2</v>
       </c>
       <c r="AJ54" s="1">
         <v>1</v>
       </c>
       <c r="AK54" s="5">
-        <v>0.012987012987012988</v>
+        <v>1.2987012987012988E-2</v>
       </c>
       <c r="AL54" s="1">
         <v>0</v>
@@ -9222,7 +9244,7 @@
         <v>1</v>
       </c>
       <c r="AW54" s="5">
-        <v>0.021739130434782608</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="AX54" s="1">
         <v>0</v>
@@ -9264,7 +9286,7 @@
         <v>1</v>
       </c>
       <c r="BK54" s="5">
-        <v>0.03125</v>
+        <v>3.125E-2</v>
       </c>
       <c r="BL54" s="1">
         <v>0</v>
@@ -9303,7 +9325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>84</v>
       </c>
@@ -9311,7 +9333,7 @@
         <v>228</v>
       </c>
       <c r="C55" s="5">
-        <v>0.168141592920354</v>
+        <v>0.16814159292035399</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -9341,13 +9363,13 @@
         <v>1</v>
       </c>
       <c r="M55" s="5">
-        <v>0.022222222222222223</v>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="N55" s="1">
         <v>4</v>
       </c>
       <c r="O55" s="5">
-        <v>0.07692307692307693</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="P55" s="1">
         <v>7</v>
@@ -9359,7 +9381,7 @@
         <v>1</v>
       </c>
       <c r="S55" s="5">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="T55" s="1">
         <v>6</v>
@@ -9377,31 +9399,31 @@
         <v>2</v>
       </c>
       <c r="Y55" s="5">
-        <v>0.041666666666666664</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="Z55" s="1">
         <v>1</v>
       </c>
       <c r="AA55" s="5">
-        <v>0.014705882352941176</v>
+        <v>1.4705882352941176E-2</v>
       </c>
       <c r="AB55" s="1">
         <v>11</v>
       </c>
       <c r="AC55" s="5">
-        <v>0.0990990990990991</v>
+        <v>9.90990990990991E-2</v>
       </c>
       <c r="AD55" s="1">
         <v>9</v>
       </c>
       <c r="AE55" s="5">
-        <v>0.0989010989010989</v>
+        <v>9.8901098901098897E-2</v>
       </c>
       <c r="AF55" s="1">
         <v>7</v>
       </c>
       <c r="AG55" s="5">
-        <v>0.2692307692307692</v>
+        <v>0.26923076923076922</v>
       </c>
       <c r="AH55" s="1">
         <v>7</v>
@@ -9425,7 +9447,7 @@
         <v>2</v>
       </c>
       <c r="AO55" s="5">
-        <v>0.0625</v>
+        <v>6.25E-2</v>
       </c>
       <c r="AP55" s="1">
         <v>8</v>
@@ -9437,7 +9459,7 @@
         <v>17</v>
       </c>
       <c r="AS55" s="5">
-        <v>0.3541666666666667</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="AT55" s="1">
         <v>10</v>
@@ -9455,7 +9477,7 @@
         <v>18</v>
       </c>
       <c r="AY55" s="5">
-        <v>0.2903225806451613</v>
+        <v>0.29032258064516131</v>
       </c>
       <c r="AZ55" s="1">
         <v>6</v>
@@ -9467,7 +9489,7 @@
         <v>20</v>
       </c>
       <c r="BC55" s="5">
-        <v>0.8695652173913043</v>
+        <v>0.86956521739130432</v>
       </c>
       <c r="BD55" s="1">
         <v>7</v>
@@ -9485,7 +9507,7 @@
         <v>9</v>
       </c>
       <c r="BI55" s="5">
-        <v>0.2571428571428571</v>
+        <v>0.25714285714285712</v>
       </c>
       <c r="BJ55" s="1">
         <v>7</v>
@@ -9530,7 +9552,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -9538,7 +9560,7 @@
         <v>3</v>
       </c>
       <c r="C56" s="5">
-        <v>0.0022123893805309734</v>
+        <v>2.2123893805309734E-3</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
@@ -9598,7 +9620,7 @@
         <v>1</v>
       </c>
       <c r="W56" s="5">
-        <v>0.02702702702702703</v>
+        <v>2.7027027027027029E-2</v>
       </c>
       <c r="X56" s="1">
         <v>0</v>
@@ -9622,7 +9644,7 @@
         <v>1</v>
       </c>
       <c r="AE56" s="5">
-        <v>0.01098901098901099</v>
+        <v>1.098901098901099E-2</v>
       </c>
       <c r="AF56" s="1">
         <v>0</v>
@@ -9640,7 +9662,7 @@
         <v>1</v>
       </c>
       <c r="AK56" s="5">
-        <v>0.012987012987012988</v>
+        <v>1.2987012987012988E-2</v>
       </c>
       <c r="AL56" s="1">
         <v>0</v>
@@ -9757,7 +9779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>86</v>
       </c>
@@ -9765,7 +9787,7 @@
         <v>78</v>
       </c>
       <c r="C57" s="5">
-        <v>0.05752212389380531</v>
+        <v>5.7522123893805309E-2</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
@@ -9813,7 +9835,7 @@
         <v>1</v>
       </c>
       <c r="S57" s="5">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="T57" s="1">
         <v>0</v>
@@ -9825,19 +9847,19 @@
         <v>1</v>
       </c>
       <c r="W57" s="5">
-        <v>0.02702702702702703</v>
+        <v>2.7027027027027029E-2</v>
       </c>
       <c r="X57" s="1">
         <v>4</v>
       </c>
       <c r="Y57" s="5">
-        <v>0.08333333333333333</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="Z57" s="1">
         <v>9</v>
       </c>
       <c r="AA57" s="5">
-        <v>0.1323529411764706</v>
+        <v>0.13235294117647059</v>
       </c>
       <c r="AB57" s="1">
         <v>15</v>
@@ -9855,7 +9877,7 @@
         <v>1</v>
       </c>
       <c r="AG57" s="5">
-        <v>0.038461538461538464</v>
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="AH57" s="1">
         <v>0</v>
@@ -9867,13 +9889,13 @@
         <v>2</v>
       </c>
       <c r="AK57" s="5">
-        <v>0.025974025974025976</v>
+        <v>2.5974025974025976E-2</v>
       </c>
       <c r="AL57" s="1">
         <v>1</v>
       </c>
       <c r="AM57" s="5">
-        <v>0.01818181818181818</v>
+        <v>1.8181818181818181E-2</v>
       </c>
       <c r="AN57" s="1">
         <v>0</v>
@@ -9885,31 +9907,31 @@
         <v>1</v>
       </c>
       <c r="AQ57" s="5">
-        <v>0.019230769230769232</v>
+        <v>1.9230769230769232E-2</v>
       </c>
       <c r="AR57" s="1">
         <v>1</v>
       </c>
       <c r="AS57" s="5">
-        <v>0.020833333333333332</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="AT57" s="1">
         <v>1</v>
       </c>
       <c r="AU57" s="5">
-        <v>0.019230769230769232</v>
+        <v>1.9230769230769232E-2</v>
       </c>
       <c r="AV57" s="1">
         <v>2</v>
       </c>
       <c r="AW57" s="5">
-        <v>0.043478260869565216</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="AX57" s="1">
         <v>1</v>
       </c>
       <c r="AY57" s="5">
-        <v>0.016129032258064516</v>
+        <v>1.6129032258064516E-2</v>
       </c>
       <c r="AZ57" s="1">
         <v>0</v>
@@ -9984,7 +10006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>87</v>
       </c>
@@ -10028,7 +10050,7 @@
         <v>7</v>
       </c>
       <c r="O58" s="5">
-        <v>0.1346153846153846</v>
+        <v>0.13461538461538461</v>
       </c>
       <c r="P58" s="1">
         <v>12</v>
@@ -10040,7 +10062,7 @@
         <v>21</v>
       </c>
       <c r="S58" s="5">
-        <v>0.525</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="T58" s="1">
         <v>16</v>
@@ -10070,7 +10092,7 @@
         <v>34</v>
       </c>
       <c r="AC58" s="5">
-        <v>0.3063063063063063</v>
+        <v>0.30630630630630629</v>
       </c>
       <c r="AD58" s="1">
         <v>24</v>
@@ -10088,7 +10110,7 @@
         <v>27</v>
       </c>
       <c r="AI58" s="5">
-        <v>0.4909090909090909</v>
+        <v>0.49090909090909091</v>
       </c>
       <c r="AJ58" s="1">
         <v>34</v>
@@ -10100,7 +10122,7 @@
         <v>28</v>
       </c>
       <c r="AM58" s="5">
-        <v>0.509090909090909</v>
+        <v>0.50909090909090904</v>
       </c>
       <c r="AN58" s="1">
         <v>18</v>
@@ -10136,7 +10158,7 @@
         <v>24</v>
       </c>
       <c r="AY58" s="5">
-        <v>0.3870967741935484</v>
+        <v>0.38709677419354838</v>
       </c>
       <c r="AZ58" s="1">
         <v>6</v>
@@ -10148,7 +10170,7 @@
         <v>2</v>
       </c>
       <c r="BC58" s="5">
-        <v>0.08695652173913043</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="BD58" s="1">
         <v>0</v>
@@ -10160,7 +10182,7 @@
         <v>7</v>
       </c>
       <c r="BG58" s="5">
-        <v>0.5384615384615384</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="BH58" s="1">
         <v>4</v>
@@ -10211,7 +10233,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -10219,7 +10241,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="5">
-        <v>0.0014749262536873156</v>
+        <v>1.4749262536873156E-3</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
@@ -10321,7 +10343,7 @@
         <v>1</v>
       </c>
       <c r="AK59" s="5">
-        <v>0.012987012987012988</v>
+        <v>1.2987012987012988E-2</v>
       </c>
       <c r="AL59" s="1">
         <v>0</v>
@@ -10357,7 +10379,7 @@
         <v>1</v>
       </c>
       <c r="AW59" s="5">
-        <v>0.021739130434782608</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="AX59" s="1">
         <v>0</v>
@@ -10438,7 +10460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>89</v>
       </c>
@@ -10446,7 +10468,7 @@
         <v>72</v>
       </c>
       <c r="C60" s="5">
-        <v>0.05309734513274336</v>
+        <v>5.3097345132743362E-2</v>
       </c>
       <c r="D60" s="1">
         <v>0</v>
@@ -10494,7 +10516,7 @@
         <v>1</v>
       </c>
       <c r="S60" s="5">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="T60" s="1">
         <v>0</v>
@@ -10512,7 +10534,7 @@
         <v>4</v>
       </c>
       <c r="Y60" s="5">
-        <v>0.08333333333333333</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="Z60" s="1">
         <v>8</v>
@@ -10530,7 +10552,7 @@
         <v>9</v>
       </c>
       <c r="AE60" s="5">
-        <v>0.0989010989010989</v>
+        <v>9.8901098901098897E-2</v>
       </c>
       <c r="AF60" s="1">
         <v>0</v>
@@ -10578,19 +10600,19 @@
         <v>1</v>
       </c>
       <c r="AU60" s="5">
-        <v>0.019230769230769232</v>
+        <v>1.9230769230769232E-2</v>
       </c>
       <c r="AV60" s="1">
         <v>1</v>
       </c>
       <c r="AW60" s="5">
-        <v>0.021739130434782608</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="AX60" s="1">
         <v>2</v>
       </c>
       <c r="AY60" s="5">
-        <v>0.03225806451612903</v>
+        <v>3.2258064516129031E-2</v>
       </c>
       <c r="AZ60" s="1">
         <v>0</v>
@@ -10626,19 +10648,19 @@
         <v>1</v>
       </c>
       <c r="BK60" s="5">
-        <v>0.03125</v>
+        <v>3.125E-2</v>
       </c>
       <c r="BL60" s="1">
         <v>1</v>
       </c>
       <c r="BM60" s="5">
-        <v>0.03333333333333333</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="BN60" s="1">
         <v>1</v>
       </c>
       <c r="BO60" s="5">
-        <v>0.020833333333333332</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="BP60" s="1">
         <v>0</v>
@@ -10656,7 +10678,7 @@
         <v>1</v>
       </c>
       <c r="BU60" s="5">
-        <v>0.06666666666666667</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="BV60" s="1">
         <v>0</v>
@@ -10665,7 +10687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>90</v>
       </c>
@@ -10892,7 +10914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>91</v>
       </c>
@@ -11119,7 +11141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>92</v>
       </c>
@@ -11127,7 +11149,7 @@
         <v>8</v>
       </c>
       <c r="C63" s="5">
-        <v>0.0058997050147492625</v>
+        <v>5.8997050147492625E-3</v>
       </c>
       <c r="D63" s="1">
         <v>0</v>
@@ -11223,19 +11245,19 @@
         <v>2</v>
       </c>
       <c r="AI63" s="5">
-        <v>0.03636363636363636</v>
+        <v>3.6363636363636362E-2</v>
       </c>
       <c r="AJ63" s="1">
         <v>1</v>
       </c>
       <c r="AK63" s="5">
-        <v>0.012987012987012988</v>
+        <v>1.2987012987012988E-2</v>
       </c>
       <c r="AL63" s="1">
         <v>2</v>
       </c>
       <c r="AM63" s="5">
-        <v>0.03636363636363636</v>
+        <v>3.6363636363636362E-2</v>
       </c>
       <c r="AN63" s="1">
         <v>0</v>
@@ -11271,7 +11293,7 @@
         <v>1</v>
       </c>
       <c r="AY63" s="5">
-        <v>0.016129032258064516</v>
+        <v>1.6129032258064516E-2</v>
       </c>
       <c r="AZ63" s="1">
         <v>0</v>
@@ -11307,13 +11329,13 @@
         <v>1</v>
       </c>
       <c r="BK63" s="5">
-        <v>0.03125</v>
+        <v>3.125E-2</v>
       </c>
       <c r="BL63" s="1">
         <v>1</v>
       </c>
       <c r="BM63" s="5">
-        <v>0.03333333333333333</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="BN63" s="1">
         <v>0</v>
@@ -11346,7 +11368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>93</v>
       </c>
@@ -11354,7 +11376,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="5">
-        <v>0.0007374631268436578</v>
+        <v>7.3746312684365781E-4</v>
       </c>
       <c r="D64" s="1">
         <v>0</v>
@@ -11564,7 +11586,7 @@
         <v>1</v>
       </c>
       <c r="BU64" s="5">
-        <v>0.06666666666666667</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="BV64" s="1">
         <v>0</v>
@@ -11573,7 +11595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>94</v>
       </c>
@@ -11800,7 +11822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>95</v>
       </c>
@@ -11808,7 +11830,7 @@
         <v>277</v>
       </c>
       <c r="C66" s="5">
-        <v>0.2042772861356932</v>
+        <v>0.20427728613569321</v>
       </c>
       <c r="D66" s="1">
         <v>0</v>
@@ -11838,7 +11860,7 @@
         <v>10</v>
       </c>
       <c r="M66" s="5">
-        <v>0.2222222222222222</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="N66" s="1">
         <v>13</v>
@@ -11874,7 +11896,7 @@
         <v>17</v>
       </c>
       <c r="Y66" s="5">
-        <v>0.3541666666666667</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="Z66" s="1">
         <v>20</v>
@@ -11898,25 +11920,25 @@
         <v>2</v>
       </c>
       <c r="AG66" s="5">
-        <v>0.07692307692307693</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="AH66" s="1">
         <v>3</v>
       </c>
       <c r="AI66" s="5">
-        <v>0.05454545454545454</v>
+        <v>5.4545454545454543E-2</v>
       </c>
       <c r="AJ66" s="1">
         <v>7</v>
       </c>
       <c r="AK66" s="5">
-        <v>0.09090909090909091</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AL66" s="1">
         <v>4</v>
       </c>
       <c r="AM66" s="5">
-        <v>0.07272727272727272</v>
+        <v>7.2727272727272724E-2</v>
       </c>
       <c r="AN66" s="1">
         <v>9</v>
@@ -11928,13 +11950,13 @@
         <v>4</v>
       </c>
       <c r="AQ66" s="5">
-        <v>0.07692307692307693</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="AR66" s="1">
         <v>3</v>
       </c>
       <c r="AS66" s="5">
-        <v>0.0625</v>
+        <v>6.25E-2</v>
       </c>
       <c r="AT66" s="1">
         <v>8</v>
@@ -11952,7 +11974,7 @@
         <v>6</v>
       </c>
       <c r="AY66" s="5">
-        <v>0.0967741935483871</v>
+        <v>9.6774193548387094E-2</v>
       </c>
       <c r="AZ66" s="1">
         <v>3</v>
@@ -11964,7 +11986,7 @@
         <v>1</v>
       </c>
       <c r="BC66" s="5">
-        <v>0.043478260869565216</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="BD66" s="1">
         <v>0</v>
@@ -11976,7 +11998,7 @@
         <v>4</v>
       </c>
       <c r="BG66" s="5">
-        <v>0.3076923076923077</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="BH66" s="1">
         <v>14</v>
@@ -12000,7 +12022,7 @@
         <v>17</v>
       </c>
       <c r="BO66" s="5">
-        <v>0.3541666666666667</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="BP66" s="1">
         <v>8</v>
@@ -12027,7 +12049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>96</v>
       </c>
@@ -12035,7 +12057,7 @@
         <v>20</v>
       </c>
       <c r="C67" s="5">
-        <v>0.014749262536873156</v>
+        <v>1.4749262536873156E-2</v>
       </c>
       <c r="D67" s="1">
         <v>0</v>
@@ -12137,7 +12159,7 @@
         <v>1</v>
       </c>
       <c r="AK67" s="5">
-        <v>0.012987012987012988</v>
+        <v>1.2987012987012988E-2</v>
       </c>
       <c r="AL67" s="1">
         <v>0</v>
@@ -12215,7 +12237,7 @@
         <v>3</v>
       </c>
       <c r="BK67" s="5">
-        <v>0.09375</v>
+        <v>9.375E-2</v>
       </c>
       <c r="BL67" s="1">
         <v>4</v>
@@ -12227,7 +12249,7 @@
         <v>4</v>
       </c>
       <c r="BO67" s="5">
-        <v>0.08333333333333333</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="BP67" s="1">
         <v>0</v>
@@ -12254,7 +12276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
         <v>97</v>
       </c>
@@ -12262,7 +12284,7 @@
         <v>8</v>
       </c>
       <c r="C68" s="8">
-        <v>0.0058997050147492625</v>
+        <v>5.8997050147492625E-3</v>
       </c>
       <c r="D68" s="7">
         <v>0</v>
@@ -12454,7 +12476,7 @@
         <v>2</v>
       </c>
       <c r="BO68" s="8">
-        <v>0.041666666666666664</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="BP68" s="7">
         <v>6</v>
@@ -12483,6 +12505,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload+read de la deuxieme collection ok
</commit_message>
<xml_diff>
--- a/statistiques_christelle-borrego_2025-05-05.xlsx
+++ b/statistiques_christelle-borrego_2025-05-05.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67572CD6-3480-469E-9951-160029460066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B88E74-4FF7-445C-BEA0-E282CE201D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,12 +346,24 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -393,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -407,6 +419,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,10 +765,10 @@
   <dimension ref="A1:BW68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="K54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="T62" sqref="T62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -917,7 +933,7 @@
       <c r="BW2" s="3"/>
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="4"/>
@@ -966,7 +982,7 @@
         <v>727</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="1">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="4"/>
@@ -1119,7 +1135,7 @@
         <v>1454</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="1">
+      <c r="D5" s="12">
         <v>1</v>
       </c>
       <c r="E5" s="4"/>
@@ -2069,7 +2085,7 @@
       <c r="BW11" s="4"/>
     </row>
     <row r="12" spans="1:75" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="4"/>
@@ -2831,7 +2847,7 @@
       <c r="BW16" s="4"/>
     </row>
     <row r="17" spans="1:75" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="4"/>
@@ -2882,7 +2898,7 @@
       <c r="C18" s="5">
         <v>0.11004126547455295</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="12">
         <v>0</v>
       </c>
       <c r="E18" s="5">
@@ -3109,7 +3125,7 @@
       <c r="C19" s="5">
         <v>1.6506189821182942E-2</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="12">
         <v>0</v>
       </c>
       <c r="E19" s="5">
@@ -3336,7 +3352,7 @@
       <c r="C20" s="5">
         <v>0.7510316368638239</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="12">
         <v>1</v>
       </c>
       <c r="E20" s="5">
@@ -3563,7 +3579,7 @@
       <c r="C21" s="5">
         <v>0.12242090784044017</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="12">
         <v>0</v>
       </c>
       <c r="E21" s="5">
@@ -3820,7 +3836,7 @@
       <c r="BW22" s="4"/>
     </row>
     <row r="23" spans="1:75" x14ac:dyDescent="0.35">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="11" t="s">
         <v>55</v>
       </c>
       <c r="C23" s="4"/>
@@ -4735,7 +4751,7 @@
       <c r="BW28" s="4"/>
     </row>
     <row r="29" spans="1:75" x14ac:dyDescent="0.35">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="11" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="4"/>

</xml_diff>